<commit_message>
Architectural Design Phase Defects Checklist
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FACULTATE\ANU 3\vvss\laburi\CheckLists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SILVIA\SEMVI\VVSS\EchipaUnu\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4F4AC5-B176-4117-82EA-51D72059C9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB6E1D2-EC16-4848-888F-D13600F52FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -146,19 +159,92 @@
   </si>
   <si>
     <t>KitchenControllerGUI.java line 16,18</t>
+  </si>
+  <si>
+    <t>Pirlea Silvia-Cristina</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>Organizararea programului este clara, exista pachete separate pentru fiecare strat al arhitecturii</t>
+  </si>
+  <si>
+    <t>Partitionarea si layering-ul este corect</t>
+  </si>
+  <si>
+    <t>Arhitectura permite realizarea tuturor cerintelor</t>
+  </si>
+  <si>
+    <t>PizzaService</t>
+  </si>
+  <si>
+    <t>La nivelul proiectului exista un singur service responabil de business layer si acesta incorporeaza toate subsistemele</t>
+  </si>
+  <si>
+    <t>Nu exista la nivelul aplicatiei o strategie de gestiune a erorilor, nu exista clase separate pentru un anumit tip de eroare. Sunt tratate doar erorile IO</t>
+  </si>
+  <si>
+    <t>MVC model este incorporat in proiect</t>
+  </si>
+  <si>
+    <t>Se acupa atat cu plata cat si cu afisarea meniului. Din numele clasei nu iti dai seama care este scopul serviciului, o denumire mai buna ar fi PizzaManagementOrdersService</t>
+  </si>
+  <si>
+    <t>Exista descriere la clase ?? Nu cred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relatiile 1 to many nu sunt bine scrise intre PaymentRepository si Payment, intre MenuGUIController si OrdersGUI ar trebui sa fie 1:10, </t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>The key entity classes are consistent with business and model layers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -337,76 +423,77 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -428,7 +515,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -774,19 +861,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -806,10 +893,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="25"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -820,10 +907,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -835,15 +922,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1030,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,19 +1137,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1075,17 +1162,21 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="17">
+        <v>235</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1096,10 +1187,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -1111,15 +1202,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1135,94 +1226,138 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E15" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
@@ -1315,7 +1450,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1336,19 +1471,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1361,7 +1496,7 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="21" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="17">
@@ -1372,14 +1507,14 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="21" t="s">
         <v>34</v>
       </c>
       <c r="J4" s="3">
@@ -1390,14 +1525,14 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="35" t="s">
+      <c r="I5" s="21" t="s">
         <v>32</v>
       </c>
       <c r="J5" s="3">
@@ -1409,15 +1544,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1683,19 +1818,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1715,8 +1850,8 @@
       <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1727,8 +1862,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -1740,8 +1875,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1971,11 +2106,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tool based analysis cu Sonarlint
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SILVIA\SEMVI\VVSS\EchipaUnu\Docs\Lab01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FACULTATE\ANU 3\vvss\github\EchipaUnu\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFF9848-03EA-4684-B2DA-2E4FF9A6E72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE9E083-E5F6-45C2-9506-1E19F5DCF4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,25 +18,12 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -152,12 +139,6 @@
     <t>KitchenControllerGUI.java line 60</t>
   </si>
   <si>
-    <t>In cod nu se verifica daca o comanda este selectata inainte de a apasa pe butonul Ready asa cum ar fi logic,ceea ce duce la o eroaredeoareceselectedOrder ar putea fi null</t>
-  </si>
-  <si>
-    <t>Unii parametri nu sunt denumiti corespunzator ,de exemplu cand vezi variabila ready in cod nu sti daca e un buton pana nu faci actiuni specifice unui buton.</t>
-  </si>
-  <si>
     <t>KitchenControllerGUI.java line 16,18</t>
   </si>
   <si>
@@ -225,6 +206,75 @@
   </si>
   <si>
     <t>Silvia Pirlea</t>
+  </si>
+  <si>
+    <t>In cod nu se verifica daca o comanda este selectata inainte de a apasa pe butonul Ready asa cum ar fi logic,ceea ce duce la o eroare deoarece selectedOrder ar putea fi null.</t>
+  </si>
+  <si>
+    <t>Unii parametri nu sunt denumiti corespunzator ,de exemplu cand vezi variabila ready in cod nu sti daca e un buton pana nu faci actiuni specifice unui buton.Parametrii ar trebui sa aibe nume cat mai sugestive legat de ceea ce reprezinta.</t>
+  </si>
+  <si>
+    <t>SonarLint</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java line 65</t>
+  </si>
+  <si>
+    <t>Metodele are trebui sa nu fie goale</t>
+  </si>
+  <si>
+    <t>OrdersGUIController avea o metoda constructor in care nu se facea nimic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A fost adaugat un comentariu inauntrul metodei </t>
+  </si>
+  <si>
+    <t>Membri statici ar trebui sa fie accesati static</t>
+  </si>
+  <si>
+    <t>In metoda setTotalAmount aveam this.totalAmount=totalAmount</t>
+  </si>
+  <si>
+    <t>this a fost inlocuit cu numele clasei</t>
+  </si>
+  <si>
+    <t>Sectiuni de cod nu ar trebui sa fie comentate</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java line 61</t>
+  </si>
+  <si>
+    <t>Bucata de cod " // = FXCollections.observableArrayList();   " era comentata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Codul comentat a fost sters </t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java line 53,109</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java line 24</t>
+  </si>
+  <si>
+    <t>Nu ar trebui folositi constructori pentrua instantia String,BigInteger etc.</t>
+  </si>
+  <si>
+    <t>extractedTableNumberString era instantiat cu =new String();</t>
+  </si>
+  <si>
+    <t>new String() a fost inlocuit cu "" reprezentat un string gol</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java line 21</t>
+  </si>
+  <si>
+    <t>Fielduri-le "public static" ar trebui sa fie constante</t>
+  </si>
+  <si>
+    <t>order era doar public si static</t>
+  </si>
+  <si>
+    <t>order a fost facut si final</t>
   </si>
 </sst>
 </file>
@@ -454,6 +504,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -496,7 +547,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Temă Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -861,19 +911,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -893,10 +943,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -907,10 +957,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -922,15 +972,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1117,7 +1167,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1137,19 +1187,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1162,8 +1212,8 @@
       <c r="H3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="36" t="s">
-        <v>62</v>
+      <c r="I3" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="J3" s="17">
         <v>235</v>
@@ -1173,10 +1223,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1187,10 +1237,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -1202,15 +1252,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -1231,11 +1281,11 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D10"/>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1243,11 +1293,11 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11"/>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1255,11 +1305,11 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1267,13 +1317,13 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
         <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1281,11 +1331,11 @@
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1293,11 +1343,11 @@
         <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1305,13 +1355,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -1319,11 +1369,11 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17"/>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1331,11 +1381,11 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -1343,11 +1393,11 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D19"/>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -1435,7 +1485,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,19 +1505,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1491,10 +1541,10 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1509,10 +1559,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -1528,15 +1578,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1563,10 +1613,10 @@
         <v>37</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1575,10 +1625,10 @@
         <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1780,8 +1830,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,19 +1852,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>29</v>
@@ -1834,8 +1884,10 @@
       <c r="C4" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="D4" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="32"/>
       <c r="H4" s="17" t="s">
         <v>20</v>
       </c>
@@ -1846,8 +1898,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="17" t="s">
         <v>21</v>
       </c>
@@ -1859,8 +1911,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1880,54 +1932,94 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
@@ -2090,11 +2182,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>